<commit_message>
Added transaction type 16 functionality
</commit_message>
<xml_diff>
--- a/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/Act1MathsEnglish.xlsx
+++ b/src/PeriodEnd/PaymentsDue/SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests/ScenarioData/Act1MathsEnglish.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\das-providerpayments\src\PeriodEnd\PaymentsDue\SFA.DAS.ProviderPayments.Calc.PaymentsDue.UnitTests\ScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{76B19010-666E-4AD6-83CC-7FBC0857AFED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6667171-F612-47F1-96C6-A7B8CA4235F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12223" firstSheet="1" activeTab="6" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="1" xr2:uid="{0D15C4CB-DC3A-4FDC-843E-A5A8882681B7}"/>
   </bookViews>
   <sheets>
     <sheet name="PastPayments" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="58">
   <si>
     <t>CommitmentId</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>19+ Apprenticeship (From May 2017) Levy Contract</t>
+  </si>
+  <si>
+    <t>TransactionType16</t>
   </si>
 </sst>
 </file>
@@ -562,29 +565,29 @@
       <selection activeCell="A2" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.3046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.84375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="46.53515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -670,76 +673,76 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="16:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P25" s="1"/>
     </row>
   </sheetData>
@@ -749,32 +752,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29113545-4422-48BA-A59E-5EDA0DBD892B}">
-  <dimension ref="A1:AC12"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AC6"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AB7" sqref="AB7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="20" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.69140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.7109375" customWidth="1"/>
+    <col min="29" max="29" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -857,13 +861,16 @@
         <v>31</v>
       </c>
       <c r="AB1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" t="s">
         <v>9</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -946,13 +953,16 @@
         <v>0</v>
       </c>
       <c r="AB2">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1035,13 +1045,16 @@
         <v>0</v>
       </c>
       <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1124,13 +1137,16 @@
         <v>0</v>
       </c>
       <c r="AB4">
-        <v>1</v>
-      </c>
-      <c r="AC4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1213,13 +1229,16 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -1302,38 +1321,41 @@
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>1</v>
-      </c>
-      <c r="AC6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="L12" s="2"/>
@@ -1352,24 +1374,24 @@
       <selection sqref="A1:AB5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.53515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="27" width="17.69140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.84375" bestFit="1" customWidth="1"/>
+    <col min="13" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1541,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1627,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1713,7 +1735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1812,16 +1834,16 @@
       <selection sqref="A1:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.15234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1844,7 +1866,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1867,7 +1889,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1890,7 +1912,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1913,7 +1935,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1936,7 +1958,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -1959,7 +1981,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1982,7 +2004,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2005,7 +2027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2028,7 +2050,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -2051,7 +2073,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -2074,7 +2096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -2097,7 +2119,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -2120,7 +2142,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -2143,7 +2165,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -2166,7 +2188,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2189,7 +2211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -2212,7 +2234,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -2235,7 +2257,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2258,7 +2280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -2281,7 +2303,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2304,7 +2326,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2327,7 +2349,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -2350,7 +2372,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2373,7 +2395,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2409,9 +2431,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2432,25 +2454,25 @@
       <selection sqref="A1:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.3828125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.53515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.3828125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2500,7 +2522,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2550,28 +2572,28 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="M7" s="2"/>
@@ -2585,19 +2607,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D57DEC8-9CE7-4F20-AF14-415D37453E52}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.07421875" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" customWidth="1"/>
-    <col min="4" max="4" width="20.53515625" customWidth="1"/>
-    <col min="5" max="5" width="21.765625" customWidth="1"/>
+    <col min="1" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -2614,7 +2636,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2017</v>
       </c>
@@ -2634,7 +2656,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2017</v>
       </c>
@@ -2654,7 +2676,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2017</v>
       </c>
@@ -2674,7 +2696,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2017</v>
       </c>
@@ -2694,7 +2716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -2714,7 +2736,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -2734,7 +2756,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2017</v>
       </c>
@@ -2754,7 +2776,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>

</xml_diff>